<commit_message>
res + maj code
</commit_message>
<xml_diff>
--- a/src/data/NAV MSCI World.xlsx
+++ b/src/data/NAV MSCI World.xlsx
@@ -8,19 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\timda\PycharmProjects\ProjetAM\src\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{648480E2-35A8-44BE-AAF4-5BDE4F9AF62A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{573276CE-082C-4E14-AEE5-785B6E6A99FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="NAV MSCI 2010" sheetId="1" r:id="rId1"/>
+    <sheet name="NAV MSCI 2007" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="2">
   <si>
     <t>Dates</t>
   </si>
@@ -32,10 +33,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
+  <numFmts count="2">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -47,17 +49,318 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Cambria"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -80,21 +383,212 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="43">
+    <cellStyle name="20 % - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20 % - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20 % - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20 % - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20 % - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20 % - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40 % - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40 % - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40 % - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40 % - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40 % - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40 % - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60 % - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60 % - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60 % - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60 % - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60 % - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60 % - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Avertissement" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Calcul" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Cellule liée" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Entrée" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Insatisfaisant" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Milliers 2" xfId="42" xr:uid="{285F8966-97C6-47BA-9A01-23F09BB5DDB6}"/>
+    <cellStyle name="Neutre" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Satisfaisant" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Sortie" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Texte explicatif" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Titre" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Titre 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Titre 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Titre 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Titre 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Vérification" xfId="13" builtinId="23" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -394,10 +888,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B214"/>
+  <dimension ref="A1:B177"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A180" workbookViewId="0">
-      <selection activeCell="I189" sqref="I189"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -416,6 +910,1439 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
+        <v>40329</v>
+      </c>
+      <c r="B2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>40359</v>
+      </c>
+      <c r="B3">
+        <v>96.798757075786739</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>40389</v>
+      </c>
+      <c r="B4">
+        <v>104.84739048971727</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>40421</v>
+      </c>
+      <c r="B5">
+        <v>101.01506544496746</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>40451</v>
+      </c>
+      <c r="B6">
+        <v>110.16138732321876</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>40480</v>
+      </c>
+      <c r="B7">
+        <v>114.59661962810678</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>40512</v>
+      </c>
+      <c r="B8">
+        <v>112.22854599103839</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>40543</v>
+      </c>
+      <c r="B9">
+        <v>120.14658040313275</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>40574</v>
+      </c>
+      <c r="B10">
+        <v>123.21332279978834</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <v>40602</v>
+      </c>
+      <c r="B11">
+        <v>127.65744485995172</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>40633</v>
+      </c>
+      <c r="B12">
+        <v>126.77330483243709</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
+        <v>40662</v>
+      </c>
+      <c r="B13">
+        <v>132.41099171968426</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <v>40694</v>
+      </c>
+      <c r="B14">
+        <v>129.98607122175497</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
+        <v>40724</v>
+      </c>
+      <c r="B15">
+        <v>128.25447211585222</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
+        <v>40753</v>
+      </c>
+      <c r="B16">
+        <v>126.32705391044358</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
+        <v>40786</v>
+      </c>
+      <c r="B17">
+        <v>117.41332840574276</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="2">
+        <v>40816</v>
+      </c>
+      <c r="B18">
+        <v>107.55653518908927</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="2">
+        <v>40847</v>
+      </c>
+      <c r="B19">
+        <v>118.17591813219155</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="2">
+        <v>40877</v>
+      </c>
+      <c r="B20">
+        <v>115.87687399986928</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="2">
+        <v>40907</v>
+      </c>
+      <c r="B21">
+        <v>116.07098407439162</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="2">
+        <v>40939</v>
+      </c>
+      <c r="B22">
+        <v>122.09293863656411</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="2">
+        <v>40968</v>
+      </c>
+      <c r="B23">
+        <v>127.95683796935243</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="2">
+        <v>40998</v>
+      </c>
+      <c r="B24">
+        <v>130.09930923400012</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="2">
+        <v>41029</v>
+      </c>
+      <c r="B25">
+        <v>128.97773644891328</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="2">
+        <v>41060</v>
+      </c>
+      <c r="B26">
+        <v>118.07634230946175</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="2">
+        <v>41089</v>
+      </c>
+      <c r="B27">
+        <v>124.08349826025342</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="2">
+        <v>41121</v>
+      </c>
+      <c r="B28">
+        <v>125.79904587924052</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="2">
+        <v>41152</v>
+      </c>
+      <c r="B29">
+        <v>129.19653086438143</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="2">
+        <v>41180</v>
+      </c>
+      <c r="B30">
+        <v>132.89521271990887</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="2">
+        <v>41213</v>
+      </c>
+      <c r="B31">
+        <v>132.3698792687174</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="2">
+        <v>41243</v>
+      </c>
+      <c r="B32">
+        <v>134.20498938092098</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="2">
+        <v>41274</v>
+      </c>
+      <c r="B33">
+        <v>137.01895686441486</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="2">
+        <v>41305</v>
+      </c>
+      <c r="B34">
+        <v>143.97981903493033</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="2">
+        <v>41333</v>
+      </c>
+      <c r="B35">
+        <v>144.36806547929476</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="2">
+        <v>41361</v>
+      </c>
+      <c r="B36">
+        <v>147.99897183002065</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="2">
+        <v>41394</v>
+      </c>
+      <c r="B37">
+        <v>153.02354687992937</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="2">
+        <v>41425</v>
+      </c>
+      <c r="B38">
+        <v>153.95514980214097</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="2">
+        <v>41453</v>
+      </c>
+      <c r="B39">
+        <v>150.32391397795365</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="2">
+        <v>41486</v>
+      </c>
+      <c r="B40">
+        <v>158.32733358391897</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="2">
+        <v>41516</v>
+      </c>
+      <c r="B41">
+        <v>155.18206568194094</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="2">
+        <v>41547</v>
+      </c>
+      <c r="B42">
+        <v>162.85230953077976</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="2">
+        <v>41578</v>
+      </c>
+      <c r="B43">
+        <v>169.40915615661095</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="2">
+        <v>41607</v>
+      </c>
+      <c r="B44">
+        <v>172.69055954183719</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" s="2">
+        <v>41639</v>
+      </c>
+      <c r="B45">
+        <v>176.44440348434549</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" s="2">
+        <v>41670</v>
+      </c>
+      <c r="B46">
+        <v>170.50925190104147</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" s="2">
+        <v>41698</v>
+      </c>
+      <c r="B47">
+        <v>178.97739829904296</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" s="2">
+        <v>41729</v>
+      </c>
+      <c r="B48">
+        <v>179.5070435989723</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="2">
+        <v>41759</v>
+      </c>
+      <c r="B49">
+        <v>181.71136587352379</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="2">
+        <v>41789</v>
+      </c>
+      <c r="B50">
+        <v>185.48786993428357</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="2">
+        <v>41820</v>
+      </c>
+      <c r="B51">
+        <v>189.04948707269179</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="2">
+        <v>41851</v>
+      </c>
+      <c r="B52">
+        <v>186.43495041649186</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" s="2">
+        <v>41880</v>
+      </c>
+      <c r="B53">
+        <v>190.59979826442347</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" s="2">
+        <v>41912</v>
+      </c>
+      <c r="B54">
+        <v>186.02066315278572</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" s="2">
+        <v>41943</v>
+      </c>
+      <c r="B55">
+        <v>187.60419682903014</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" s="2">
+        <v>41971</v>
+      </c>
+      <c r="B56">
+        <v>191.74946460132139</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" s="2">
+        <v>42004</v>
+      </c>
+      <c r="B57">
+        <v>188.98608906498481</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" s="2">
+        <v>42034</v>
+      </c>
+      <c r="B58">
+        <v>186.23283433176232</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" s="2">
+        <v>42062</v>
+      </c>
+      <c r="B59">
+        <v>196.77629630800055</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" s="2">
+        <v>42094</v>
+      </c>
+      <c r="B60">
+        <v>194.25896071298158</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" s="2">
+        <v>42124</v>
+      </c>
+      <c r="B61">
+        <v>199.3078780979468</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" s="2">
+        <v>42153</v>
+      </c>
+      <c r="B62">
+        <v>200.50857214264326</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" s="2">
+        <v>42185</v>
+      </c>
+      <c r="B63">
+        <v>196.00138259374899</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" s="2">
+        <v>42216</v>
+      </c>
+      <c r="B64">
+        <v>200.04224233737563</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" s="2">
+        <v>42247</v>
+      </c>
+      <c r="B65">
+        <v>187.26256317904657</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" s="2">
+        <v>42277</v>
+      </c>
+      <c r="B66">
+        <v>180.96514485479491</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" s="2">
+        <v>42307</v>
+      </c>
+      <c r="B67">
+        <v>194.77954253597025</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" s="2">
+        <v>42338</v>
+      </c>
+      <c r="B68">
+        <v>194.25741627595633</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69" s="2">
+        <v>42369</v>
+      </c>
+      <c r="B69">
+        <v>191.28653017186355</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70" s="2">
+        <v>42398</v>
+      </c>
+      <c r="B70">
+        <v>180.43066151162668</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71" s="2">
+        <v>42429</v>
+      </c>
+      <c r="B71">
+        <v>179.57239493490204</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72" s="2">
+        <v>42460</v>
+      </c>
+      <c r="B72">
+        <v>191.52449299643251</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73" s="2">
+        <v>42489</v>
+      </c>
+      <c r="B73">
+        <v>195.06050037475262</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74" s="2">
+        <v>42521</v>
+      </c>
+      <c r="B74">
+        <v>196.59704827008875</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75" s="2">
+        <v>42551</v>
+      </c>
+      <c r="B75">
+        <v>195.03528800822335</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76" s="2">
+        <v>42580</v>
+      </c>
+      <c r="B76">
+        <v>203.4621841969979</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77" s="2">
+        <v>42613</v>
+      </c>
+      <c r="B77">
+        <v>204.15023490693241</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78" s="2">
+        <v>42643</v>
+      </c>
+      <c r="B78">
+        <v>205.43560680851769</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79" s="2">
+        <v>42674</v>
+      </c>
+      <c r="B79">
+        <v>202.09339834460403</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80" s="2">
+        <v>42704</v>
+      </c>
+      <c r="B80">
+        <v>205.75907768969284</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81" s="2">
+        <v>42734</v>
+      </c>
+      <c r="B81">
+        <v>210.7942966500481</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82" s="2">
+        <v>42766</v>
+      </c>
+      <c r="B82">
+        <v>216.24819576833386</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83" s="2">
+        <v>42794</v>
+      </c>
+      <c r="B83">
+        <v>222.15025633027156</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84" s="2">
+        <v>42825</v>
+      </c>
+      <c r="B84">
+        <v>225.25527175737227</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85" s="2">
+        <v>42853</v>
+      </c>
+      <c r="B85">
+        <v>228.96050159953924</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86" s="2">
+        <v>42886</v>
+      </c>
+      <c r="B86">
+        <v>234.29261096040412</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87" s="2">
+        <v>42916</v>
+      </c>
+      <c r="B87">
+        <v>235.81988065090363</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88" s="2">
+        <v>42947</v>
+      </c>
+      <c r="B88">
+        <v>241.81252510042239</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89" s="2">
+        <v>42978</v>
+      </c>
+      <c r="B89">
+        <v>242.5627165547009</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A90" s="2">
+        <v>43007</v>
+      </c>
+      <c r="B90">
+        <v>248.11062842705883</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A91" s="2">
+        <v>43039</v>
+      </c>
+      <c r="B91">
+        <v>253.36411070959969</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A92" s="2">
+        <v>43069</v>
+      </c>
+      <c r="B92">
+        <v>259.07006200168416</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A93" s="2">
+        <v>43098</v>
+      </c>
+      <c r="B93">
+        <v>263.04521026847732</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A94" s="2">
+        <v>43131</v>
+      </c>
+      <c r="B94">
+        <v>276.74513615720969</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A95" s="2">
+        <v>43159</v>
+      </c>
+      <c r="B95">
+        <v>265.96556350954432</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A96" s="2">
+        <v>43188</v>
+      </c>
+      <c r="B96">
+        <v>261.19209537393601</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A97" s="2">
+        <v>43220</v>
+      </c>
+      <c r="B97">
+        <v>264.38782633712918</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A98" s="2">
+        <v>43251</v>
+      </c>
+      <c r="B98">
+        <v>267.00519935034851</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A99" s="2">
+        <v>43280</v>
+      </c>
+      <c r="B99">
+        <v>267.34999077319208</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A100" s="2">
+        <v>43312</v>
+      </c>
+      <c r="B100">
+        <v>275.77741034148102</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A101" s="2">
+        <v>43343</v>
+      </c>
+      <c r="B101">
+        <v>279.66047090525404</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A102" s="2">
+        <v>43371</v>
+      </c>
+      <c r="B102">
+        <v>281.78560478873356</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A103" s="2">
+        <v>43404</v>
+      </c>
+      <c r="B103">
+        <v>260.97035396630429</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A104" s="2">
+        <v>43434</v>
+      </c>
+      <c r="B104">
+        <v>265.25291605187027</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A105" s="2">
+        <v>43465</v>
+      </c>
+      <c r="B105">
+        <v>245.1368652739373</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A106" s="2">
+        <v>43496</v>
+      </c>
+      <c r="B106">
+        <v>263.85958099778281</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A107" s="2">
+        <v>43524</v>
+      </c>
+      <c r="B107">
+        <v>272.34636666867266</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A108" s="2">
+        <v>43553</v>
+      </c>
+      <c r="B108">
+        <v>276.65678820173554</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A109" s="2">
+        <v>43585</v>
+      </c>
+      <c r="B109">
+        <v>287.05566082059084</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A110" s="2">
+        <v>43616</v>
+      </c>
+      <c r="B110">
+        <v>271.42217301650976</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A111" s="2">
+        <v>43644</v>
+      </c>
+      <c r="B111">
+        <v>288.64732025228443</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A112" s="2">
+        <v>43677</v>
+      </c>
+      <c r="B112">
+        <v>290.18760676126334</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A113" s="2">
+        <v>43707</v>
+      </c>
+      <c r="B113">
+        <v>285.45884969868217</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A114" s="2">
+        <v>43738</v>
+      </c>
+      <c r="B114">
+        <v>291.97292604552842</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A115" s="2">
+        <v>43769</v>
+      </c>
+      <c r="B115">
+        <v>299.85085910204816</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A116" s="2">
+        <v>43798</v>
+      </c>
+      <c r="B116">
+        <v>308.62521196701982</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A117" s="2">
+        <v>43830</v>
+      </c>
+      <c r="B117">
+        <v>317.97675268986495</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A118" s="2">
+        <v>43861</v>
+      </c>
+      <c r="B118">
+        <v>317.04575512229275</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A119" s="2">
+        <v>43889</v>
+      </c>
+      <c r="B119">
+        <v>290.29469442875734</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A120" s="2">
+        <v>43921</v>
+      </c>
+      <c r="B120">
+        <v>252.73437117408636</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A121" s="2">
+        <v>43951</v>
+      </c>
+      <c r="B121">
+        <v>279.14347276646851</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A122" s="2">
+        <v>43980</v>
+      </c>
+      <c r="B122">
+        <v>293.51380401659736</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A123" s="2">
+        <v>44012</v>
+      </c>
+      <c r="B123">
+        <v>302.1162362932086</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A124" s="2">
+        <v>44043</v>
+      </c>
+      <c r="B124">
+        <v>316.5120508262126</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A125" s="2">
+        <v>44074</v>
+      </c>
+      <c r="B125">
+        <v>338.21649805917434</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A126" s="2">
+        <v>44104</v>
+      </c>
+      <c r="B126">
+        <v>327.50281088818087</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A127" s="2">
+        <v>44134</v>
+      </c>
+      <c r="B127">
+        <v>318.32101637465121</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A128" s="2">
+        <v>44165</v>
+      </c>
+      <c r="B128">
+        <v>357.89545767273648</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A129" s="2">
+        <v>44196</v>
+      </c>
+      <c r="B129">
+        <v>373.53874985349057</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A130" s="2">
+        <v>44225</v>
+      </c>
+      <c r="B130">
+        <v>370.78557054253088</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A131" s="2">
+        <v>44253</v>
+      </c>
+      <c r="B131">
+        <v>381.64491649136028</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A132" s="2">
+        <v>44286</v>
+      </c>
+      <c r="B132">
+        <v>395.49704320748532</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A133" s="2">
+        <v>44316</v>
+      </c>
+      <c r="B133">
+        <v>414.01091965790187</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A134" s="2">
+        <v>44347</v>
+      </c>
+      <c r="B134">
+        <v>420.73713483768131</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A135" s="2">
+        <v>44377</v>
+      </c>
+      <c r="B135">
+        <v>427.86315307674272</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A136" s="2">
+        <v>44407</v>
+      </c>
+      <c r="B136">
+        <v>436.1812153424404</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A137" s="2">
+        <v>44439</v>
+      </c>
+      <c r="B137">
+        <v>447.8264090303378</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A138" s="2">
+        <v>44469</v>
+      </c>
+      <c r="B138">
+        <v>430.45266588450983</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A139" s="2">
+        <v>44498</v>
+      </c>
+      <c r="B139">
+        <v>455.4217237086234</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A140" s="2">
+        <v>44530</v>
+      </c>
+      <c r="B140">
+        <v>447.45691202917828</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A141" s="2">
+        <v>44561</v>
+      </c>
+      <c r="B141">
+        <v>466.29446078736805</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A142" s="2">
+        <v>44592</v>
+      </c>
+      <c r="B142">
+        <v>443.2885154921039</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A143" s="2">
+        <v>44620</v>
+      </c>
+      <c r="B143">
+        <v>433.56435257697615</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A144" s="2">
+        <v>44651</v>
+      </c>
+      <c r="B144">
+        <v>446.07482668881477</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A145" s="2">
+        <v>44680</v>
+      </c>
+      <c r="B145">
+        <v>409.94738184390712</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A146" s="2">
+        <v>44712</v>
+      </c>
+      <c r="B146">
+        <v>412.11464705518318</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A147" s="2">
+        <v>44742</v>
+      </c>
+      <c r="B147">
+        <v>376.60068182893633</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A148" s="2">
+        <v>44771</v>
+      </c>
+      <c r="B148">
+        <v>406.76105200865192</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A149" s="2">
+        <v>44804</v>
+      </c>
+      <c r="B149">
+        <v>390.14712100057034</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A150" s="2">
+        <v>44834</v>
+      </c>
+      <c r="B150">
+        <v>353.59128038829869</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A151" s="2">
+        <v>44865</v>
+      </c>
+      <c r="B151">
+        <v>379.64611072912192</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A152" s="2">
+        <v>44895</v>
+      </c>
+      <c r="B152">
+        <v>407.52852035071697</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A153" s="2">
+        <v>44925</v>
+      </c>
+      <c r="B153">
+        <v>390.18462987230254</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A154" s="2">
+        <v>44957</v>
+      </c>
+      <c r="B154">
+        <v>417.85715289648948</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A155" s="2">
+        <v>44985</v>
+      </c>
+      <c r="B155">
+        <v>408.33018650403181</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A156" s="2">
+        <v>45016</v>
+      </c>
+      <c r="B156">
+        <v>422.86166730060188</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A157" s="2">
+        <v>45044</v>
+      </c>
+      <c r="B157">
+        <v>430.89315849519443</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A158" s="2">
+        <v>45077</v>
+      </c>
+      <c r="B158">
+        <v>430.06248909562731</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A159" s="2">
+        <v>45107</v>
+      </c>
+      <c r="B159">
+        <v>455.79109007168</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A160" s="2">
+        <v>45138</v>
+      </c>
+      <c r="B160">
+        <v>471.16135864947927</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A161" s="2">
+        <v>45169</v>
+      </c>
+      <c r="B161">
+        <v>461.17839859832617</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A162" s="2">
+        <v>45198</v>
+      </c>
+      <c r="B162">
+        <v>441.69678067365629</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A163" s="2">
+        <v>45230</v>
+      </c>
+      <c r="B163">
+        <v>430.29630669883738</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A164" s="2">
+        <v>45260</v>
+      </c>
+      <c r="B164">
+        <v>469.53558191688967</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A165" s="2">
+        <v>45289</v>
+      </c>
+      <c r="B165">
+        <v>493.20761779304786</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A166" s="2">
+        <v>45322</v>
+      </c>
+      <c r="B166">
+        <v>500.01198661977446</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A167" s="2">
+        <v>45351</v>
+      </c>
+      <c r="B167">
+        <v>523.49410140345844</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A168" s="2">
+        <v>45379</v>
+      </c>
+      <c r="B168">
+        <v>541.29013905096519</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A169" s="2">
+        <v>45412</v>
+      </c>
+      <c r="B169">
+        <v>521.78439430429376</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A170" s="2">
+        <v>45443</v>
+      </c>
+      <c r="B170">
+        <v>546.44537708169787</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A171" s="2">
+        <v>45471</v>
+      </c>
+      <c r="B171">
+        <v>559.31467272062241</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A172" s="2">
+        <v>45504</v>
+      </c>
+      <c r="B172">
+        <v>570.77018535632624</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A173" s="2">
+        <v>45534</v>
+      </c>
+      <c r="B173">
+        <v>586.32843692338383</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A174" s="2">
+        <v>45565</v>
+      </c>
+      <c r="B174">
+        <v>597.79934950566746</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A175" s="2">
+        <v>45596</v>
+      </c>
+      <c r="B175">
+        <v>588.25325909220089</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A176" s="2">
+        <v>45625</v>
+      </c>
+      <c r="B176">
+        <v>616.65703469222694</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A177" s="2">
+        <v>45657</v>
+      </c>
+      <c r="B177">
+        <v>602.65308215782693</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21DD0443-E1D8-46B1-BA55-FF1D7CE692E9}">
+  <dimension ref="A1:B214"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
         <v>39202</v>
       </c>
       <c r="B2">
@@ -2119,6 +4046,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>